<commit_message>
ajout encryptedPassword + ajout autres eleves CSV
</commit_message>
<xml_diff>
--- a/Documents/Eleves.xlsx
+++ b/Documents/Eleves.xlsx
@@ -3,7 +3,7 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="21001"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2A30D691-366D-42C0-BC33-435647AB2B57}" xr6:coauthVersionLast="38" xr6:coauthVersionMax="38" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9074E7AB-FBE4-4FCF-813D-542DF9834107}" xr6:coauthVersionLast="38" xr6:coauthVersionMax="38" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12645" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="15" uniqueCount="15">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="27" uniqueCount="27">
   <si>
     <t xml:space="preserve">Nom	</t>
   </si>
@@ -65,16 +65,60 @@
   </si>
   <si>
     <t>Liboutet.Nathan@gmail.com</t>
+  </si>
+  <si>
+    <t>Lorthioir</t>
+  </si>
+  <si>
+    <t>Jérémy</t>
+  </si>
+  <si>
+    <t>Lorthioir.Jeremy@etu.unilim.fr</t>
+  </si>
+  <si>
+    <t>Sparrow</t>
+  </si>
+  <si>
+    <t>Jack</t>
+  </si>
+  <si>
+    <t>Sparrow.Jack@pirate.com</t>
+  </si>
+  <si>
+    <t>Potter</t>
+  </si>
+  <si>
+    <t>Harry</t>
+  </si>
+  <si>
+    <t>HarryPotter@poudlard.com</t>
+  </si>
+  <si>
+    <t>Picsou</t>
+  </si>
+  <si>
+    <t>Balthazar</t>
+  </si>
+  <si>
+    <t>Balthazar.Picsou@riche.com</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="1" x14ac:knownFonts="1">
+  <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color theme="10"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -97,13 +141,16 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="1">
+  <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="1"/>
   </cellXfs>
-  <cellStyles count="1">
+  <cellStyles count="2">
+    <cellStyle name="Lien hypertexte" xfId="1" builtinId="8"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -382,10 +429,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:C5"/>
+  <dimension ref="A1:C9"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C7" sqref="C7"/>
+      <selection activeCell="A10" sqref="A10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -449,7 +496,57 @@
         <v>14</v>
       </c>
     </row>
+    <row r="6" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A6" t="s">
+        <v>15</v>
+      </c>
+      <c r="B6" t="s">
+        <v>16</v>
+      </c>
+      <c r="C6" s="1" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="7" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A7" t="s">
+        <v>18</v>
+      </c>
+      <c r="B7" t="s">
+        <v>19</v>
+      </c>
+      <c r="C7" s="1" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="8" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A8" t="s">
+        <v>21</v>
+      </c>
+      <c r="B8" t="s">
+        <v>22</v>
+      </c>
+      <c r="C8" s="1" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="9" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A9" t="s">
+        <v>24</v>
+      </c>
+      <c r="B9" t="s">
+        <v>25</v>
+      </c>
+      <c r="C9" s="1" t="s">
+        <v>26</v>
+      </c>
+    </row>
   </sheetData>
+  <hyperlinks>
+    <hyperlink ref="C6" r:id="rId1" xr:uid="{8C690AF2-813E-4E8D-ACF8-8CF8CAC3E60A}"/>
+    <hyperlink ref="C7" r:id="rId2" xr:uid="{AF0A467D-7ACC-463B-85E8-EDD928282000}"/>
+    <hyperlink ref="C8" r:id="rId3" xr:uid="{DF3FC5A3-BED1-441B-9587-AB6566384066}"/>
+    <hyperlink ref="C9" r:id="rId4" xr:uid="{434F8554-93AF-400A-9E25-B03B32068275}"/>
+  </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
</xml_diff>